<commit_message>
added reaming testcases for login
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,6 +520,305 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TC_LOGIN_02</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Login with valid email and invalid password</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1. Enter valid email
+2. Enter invalid password
+3. Click Login</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Email:superadmin
+Password:admin</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Error message should be displayed</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Expected: Error message should be displayed | Actual: Locator expected to be visible
+Actual value: &lt;element(s) not found&gt; 
+Call log:
+  - Expect "to_be_visible" with timeout 5000ms
+  - waiting for locator(".error, .error-message, .alert-danger, .validation-error")
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TC_LOGIN_03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Login with invalid email and valid password</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1. Enter invalid email
+2. Enter valid password
+3. Click Login</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Email:super
+Password:superadmin</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Error message should be displayed</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Expected: Error message should be displayed | Actual: Locator expected to be visible
+Actual value: &lt;element(s) not found&gt; 
+Call log:
+  - Expect "to_be_visible" with timeout 5000ms
+  - waiting for locator(".error, .error-message, .alert-danger, .validation-error")
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TC_LOGIN_04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Login with invalid email and invalid password</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1. Enter invalid email
+2. Enter invalid password
+3. Click Login</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Email:superadmin
+Password:superadmin</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Error message should be displayed</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Expected: Error message should be displayed | Actual: Locator expected to be visible
+Actual value: &lt;element(s) not found&gt; 
+Call log:
+  - Expect "to_be_visible" with timeout 5000ms
+  - waiting for locator(".error, .error-message, .alert-danger, .validation-error")
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TC_LOGIN_05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Login with empty email and empty password</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1. Leave fields empty
+2. Click Login</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Email:superadmin
+Password:superadmin</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Validation message should be shown</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Expected: Validation message should be shown | Actual: Locator expected to be visible
+Actual value: &lt;element(s) not found&gt; 
+Call log:
+  - Expect "to_be_visible" with timeout 5000ms
+  - waiting for locator(".error, .error-message, .alert-danger, .validation-error")
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TC_LOGIN_06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Login with empty email</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1. Leave email empty
+2. Enter password
+3. Click Login</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Email:superadmin
+Password:superadmin</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Email required validation should appear</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Expected: Email required validation should appear | Actual: Locator expected to be visible
+Actual value: &lt;element(s) not found&gt; 
+Call log:
+  - Expect "to_be_visible" with timeout 5000ms
+  - waiting for locator(".error, .error-message, .alert-danger, .validation-error")
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TC_LOGIN_07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Login with empty password</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1. Enter email
+2. Leave password empty
+3. Click Login</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Email:superadmin
+Password:superadmin</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Password required validation should appear</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Expected: Password required validation should appear | Actual: Locator expected to be visible
+Actual value: &lt;element(s) not found&gt; 
+Call log:
+  - Expect "to_be_visible" with timeout 5000ms
+  - waiting for locator(".error, .error-message, .alert-danger, .validation-error")
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>